<commit_message>
142 Update UI Design
</commit_message>
<xml_diff>
--- a/GameMaster/GameDesign/进度.xlsx
+++ b/GameMaster/GameDesign/进度.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\建造工程\Project\GameMaster\GameDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66C953D-4412-4F25-A640-9DE2AB5C002D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9E8823-27D5-4071-97E6-311A2687E454}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="75">
   <si>
     <t>装入unity</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -310,6 +310,22 @@
   </si>
   <si>
     <t>AssemblePartChooseDialog</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>含模板选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AssembleShipDesignPage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部件装配工厂</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造船厂</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -379,7 +395,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -491,11 +507,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color indexed="64"/>
+      </left>
+      <right style="hair">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -573,6 +615,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -923,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AR68"/>
+  <dimension ref="A1:AR71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1156,7 +1204,7 @@
       <c r="G16" s="26"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -1165,105 +1213,238 @@
       <c r="G17" s="26"/>
       <c r="H17" s="18"/>
     </row>
-    <row r="18" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="26" t="s">
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="H18" s="18"/>
-    </row>
-    <row r="19" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="26"/>
+      <c r="H18" s="29"/>
+    </row>
+    <row r="19" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9"/>
+      <c r="B19" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
       <c r="H19" s="18"/>
-    </row>
-    <row r="20" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
+      <c r="R19" s="10"/>
+      <c r="S19" s="10"/>
+      <c r="T19" s="10"/>
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="10"/>
+      <c r="AH19" s="10"/>
+      <c r="AI19" s="10"/>
+      <c r="AJ19" s="10"/>
+      <c r="AK19" s="10"/>
+      <c r="AL19" s="10"/>
+      <c r="AM19" s="10"/>
+      <c r="AN19" s="10"/>
+      <c r="AO19" s="10"/>
+      <c r="AP19" s="10"/>
+      <c r="AQ19" s="10"/>
+      <c r="AR19" s="10"/>
+    </row>
+    <row r="20" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="9"/>
+      <c r="B20" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
+      <c r="P20" s="10"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+      <c r="T20" s="10"/>
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="10"/>
+      <c r="AI20" s="10"/>
+      <c r="AJ20" s="10"/>
+      <c r="AK20" s="10"/>
+      <c r="AL20" s="10"/>
+      <c r="AM20" s="10"/>
+      <c r="AN20" s="10"/>
+      <c r="AO20" s="10"/>
+      <c r="AP20" s="10"/>
+      <c r="AQ20" s="10"/>
+      <c r="AR20" s="10"/>
+    </row>
+    <row r="21" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="9"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
+      <c r="P21" s="10"/>
+      <c r="Q21" s="10"/>
+      <c r="R21" s="10"/>
+      <c r="S21" s="10"/>
+      <c r="T21" s="10"/>
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AH21" s="10"/>
+      <c r="AI21" s="10"/>
+      <c r="AJ21" s="10"/>
+      <c r="AK21" s="10"/>
+      <c r="AL21" s="10"/>
+      <c r="AM21" s="10"/>
+      <c r="AN21" s="10"/>
+      <c r="AO21" s="10"/>
+      <c r="AP21" s="10"/>
+      <c r="AQ21" s="10"/>
+      <c r="AR21" s="10"/>
+    </row>
+    <row r="22" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="9"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="10"/>
+      <c r="T22" s="10"/>
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="10"/>
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
+      <c r="AH22" s="10"/>
+      <c r="AI22" s="10"/>
+      <c r="AJ22" s="10"/>
+      <c r="AK22" s="10"/>
+      <c r="AL22" s="10"/>
+      <c r="AM22" s="10"/>
+      <c r="AN22" s="10"/>
+      <c r="AO22" s="10"/>
+      <c r="AP22" s="10"/>
+      <c r="AQ22" s="10"/>
+      <c r="AR22" s="10"/>
+    </row>
+    <row r="23" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B23" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="18" t="s">
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="30" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="4"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="18"/>
-    </row>
-    <row r="22" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="18"/>
-    </row>
-    <row r="24" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="6"/>
+    <row r="24" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="5"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
+      <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="26"/>
-      <c r="H24" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H24" s="18"/>
+    </row>
+    <row r="25" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="5"/>
@@ -1271,12 +1452,15 @@
       <c r="F25" s="5"/>
       <c r="G25" s="26"/>
       <c r="H25" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="B26" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1285,31 +1469,42 @@
       <c r="G26" s="26"/>
       <c r="H26" s="18"/>
     </row>
-    <row r="27" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="4"/>
-      <c r="C27" s="5"/>
+    <row r="27" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="6"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="E27" s="6"/>
       <c r="F27" s="5"/>
       <c r="G27" s="26"/>
-      <c r="H27" s="18"/>
-    </row>
-    <row r="28" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H27" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="C28" s="6"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="E28" s="6"/>
       <c r="F28" s="5"/>
       <c r="G28" s="26"/>
-      <c r="H28" s="18"/>
-    </row>
-    <row r="29" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="4"/>
+      <c r="H28" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -1317,7 +1512,7 @@
       <c r="G29" s="26"/>
       <c r="H29" s="18"/>
     </row>
-    <row r="30" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -1326,181 +1521,75 @@
       <c r="G30" s="26"/>
       <c r="H30" s="18"/>
     </row>
-    <row r="31" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="C31" s="5"/>
       <c r="D31" s="5"/>
-      <c r="E31" s="6"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="26"/>
-      <c r="H31" s="18" t="s">
+      <c r="H31" s="18"/>
+    </row>
+    <row r="32" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="18"/>
+    </row>
+    <row r="33" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="18"/>
+    </row>
+    <row r="34" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="12" t="s">
+    <row r="35" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="27"/>
-      <c r="H32" s="18" t="s">
+      <c r="C35" s="13"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="18" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="33" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="B33" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="10"/>
-      <c r="U33" s="10"/>
-      <c r="V33" s="10"/>
-      <c r="W33" s="10"/>
-      <c r="X33" s="10"/>
-      <c r="Y33" s="10"/>
-      <c r="Z33" s="10"/>
-      <c r="AA33" s="10"/>
-      <c r="AB33" s="10"/>
-      <c r="AC33" s="10"/>
-      <c r="AD33" s="10"/>
-      <c r="AE33" s="10"/>
-      <c r="AF33" s="10"/>
-      <c r="AG33" s="10"/>
-      <c r="AH33" s="10"/>
-      <c r="AI33" s="10"/>
-      <c r="AJ33" s="10"/>
-      <c r="AK33" s="10"/>
-      <c r="AL33" s="10"/>
-      <c r="AM33" s="10"/>
-      <c r="AN33" s="10"/>
-      <c r="AO33" s="10"/>
-      <c r="AP33" s="10"/>
-      <c r="AQ33" s="10"/>
-      <c r="AR33" s="10"/>
-    </row>
-    <row r="34" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="18"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="10"/>
-      <c r="U34" s="10"/>
-      <c r="V34" s="10"/>
-      <c r="W34" s="10"/>
-      <c r="X34" s="10"/>
-      <c r="Y34" s="10"/>
-      <c r="Z34" s="10"/>
-      <c r="AA34" s="10"/>
-      <c r="AB34" s="10"/>
-      <c r="AC34" s="10"/>
-      <c r="AD34" s="10"/>
-      <c r="AE34" s="10"/>
-      <c r="AF34" s="10"/>
-      <c r="AG34" s="10"/>
-      <c r="AH34" s="10"/>
-      <c r="AI34" s="10"/>
-      <c r="AJ34" s="10"/>
-      <c r="AK34" s="10"/>
-      <c r="AL34" s="10"/>
-      <c r="AM34" s="10"/>
-      <c r="AN34" s="10"/>
-      <c r="AO34" s="10"/>
-      <c r="AP34" s="10"/>
-      <c r="AQ34" s="10"/>
-      <c r="AR34" s="10"/>
-    </row>
-    <row r="35" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="10"/>
-      <c r="T35" s="10"/>
-      <c r="U35" s="10"/>
-      <c r="V35" s="10"/>
-      <c r="W35" s="10"/>
-      <c r="X35" s="10"/>
-      <c r="Y35" s="10"/>
-      <c r="Z35" s="10"/>
-      <c r="AA35" s="10"/>
-      <c r="AB35" s="10"/>
-      <c r="AC35" s="10"/>
-      <c r="AD35" s="10"/>
-      <c r="AE35" s="10"/>
-      <c r="AF35" s="10"/>
-      <c r="AG35" s="10"/>
-      <c r="AH35" s="10"/>
-      <c r="AI35" s="10"/>
-      <c r="AJ35" s="10"/>
-      <c r="AK35" s="10"/>
-      <c r="AL35" s="10"/>
-      <c r="AM35" s="10"/>
-      <c r="AN35" s="10"/>
-      <c r="AO35" s="10"/>
-      <c r="AP35" s="10"/>
-      <c r="AQ35" s="10"/>
-      <c r="AR35" s="10"/>
     </row>
     <row r="36" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="19"/>
+      <c r="B36" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="23"/>
       <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
+      <c r="E36" s="23"/>
       <c r="F36" s="19"/>
       <c r="G36" s="28"/>
       <c r="H36" s="18"/>
@@ -1541,62 +1630,168 @@
       <c r="AQ36" s="10"/>
       <c r="AR36" s="10"/>
     </row>
-    <row r="37" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="9"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="10"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="10"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="10"/>
+      <c r="U37" s="10"/>
+      <c r="V37" s="10"/>
+      <c r="W37" s="10"/>
+      <c r="X37" s="10"/>
+      <c r="Y37" s="10"/>
+      <c r="Z37" s="10"/>
+      <c r="AA37" s="10"/>
+      <c r="AB37" s="10"/>
+      <c r="AC37" s="10"/>
+      <c r="AD37" s="10"/>
+      <c r="AE37" s="10"/>
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="10"/>
+      <c r="AH37" s="10"/>
+      <c r="AI37" s="10"/>
+      <c r="AJ37" s="10"/>
+      <c r="AK37" s="10"/>
+      <c r="AL37" s="10"/>
+      <c r="AM37" s="10"/>
+      <c r="AN37" s="10"/>
+      <c r="AO37" s="10"/>
+      <c r="AP37" s="10"/>
+      <c r="AQ37" s="10"/>
+      <c r="AR37" s="10"/>
+    </row>
+    <row r="38" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="9"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="18"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+      <c r="O38" s="10"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="10"/>
+      <c r="U38" s="10"/>
+      <c r="V38" s="10"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="10"/>
+      <c r="Y38" s="10"/>
+      <c r="Z38" s="10"/>
+      <c r="AA38" s="10"/>
+      <c r="AB38" s="10"/>
+      <c r="AC38" s="10"/>
+      <c r="AD38" s="10"/>
+      <c r="AE38" s="10"/>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="10"/>
+      <c r="AH38" s="10"/>
+      <c r="AI38" s="10"/>
+      <c r="AJ38" s="10"/>
+      <c r="AK38" s="10"/>
+      <c r="AL38" s="10"/>
+      <c r="AM38" s="10"/>
+      <c r="AN38" s="10"/>
+      <c r="AO38" s="10"/>
+      <c r="AP38" s="10"/>
+      <c r="AQ38" s="10"/>
+      <c r="AR38" s="10"/>
+    </row>
+    <row r="39" spans="1:44" s="11" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="9"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="18"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="10"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
+      <c r="W39" s="10"/>
+      <c r="X39" s="10"/>
+      <c r="Y39" s="10"/>
+      <c r="Z39" s="10"/>
+      <c r="AA39" s="10"/>
+      <c r="AB39" s="10"/>
+      <c r="AC39" s="10"/>
+      <c r="AD39" s="10"/>
+      <c r="AE39" s="10"/>
+      <c r="AF39" s="10"/>
+      <c r="AG39" s="10"/>
+      <c r="AH39" s="10"/>
+      <c r="AI39" s="10"/>
+      <c r="AJ39" s="10"/>
+      <c r="AK39" s="10"/>
+      <c r="AL39" s="10"/>
+      <c r="AM39" s="10"/>
+      <c r="AN39" s="10"/>
+      <c r="AO39" s="10"/>
+      <c r="AP39" s="10"/>
+      <c r="AQ39" s="10"/>
+      <c r="AR39" s="10"/>
+    </row>
+    <row r="40" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B40" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="18" t="s">
+      <c r="C40" s="16"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+    <row r="41" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="26"/>
-      <c r="H38" s="18"/>
-    </row>
-    <row r="39" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="18"/>
-    </row>
-    <row r="40" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="4"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="26"/>
-      <c r="H40" s="18"/>
-    </row>
-    <row r="41" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="4"/>
-      <c r="C41" s="5"/>
+      <c r="C41" s="6"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -1604,7 +1799,12 @@
       <c r="H41" s="18"/>
     </row>
     <row r="42" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="4"/>
+      <c r="A42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
@@ -1631,130 +1831,121 @@
       <c r="H44" s="18"/>
     </row>
     <row r="45" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C45" s="6"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="5"/>
       <c r="D45" s="5"/>
-      <c r="E45" s="6"/>
+      <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="26"/>
       <c r="H45" s="18"/>
     </row>
     <row r="46" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C46" s="6"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="6"/>
+      <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="26"/>
       <c r="H46" s="18"/>
     </row>
     <row r="47" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="6"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="6"/>
+      <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="26"/>
-      <c r="H47" s="18" t="s">
-        <v>66</v>
-      </c>
+      <c r="H47" s="18"/>
     </row>
     <row r="48" spans="1:44" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="4"/>
-      <c r="C48" s="5"/>
+      <c r="A48" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="6"/>
       <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
+      <c r="E48" s="6"/>
       <c r="F48" s="5"/>
       <c r="G48" s="26"/>
       <c r="H48" s="18"/>
     </row>
     <row r="49" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="4"/>
-      <c r="C49" s="5"/>
+      <c r="A49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="6"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="E49" s="6"/>
       <c r="F49" s="5"/>
       <c r="G49" s="26"/>
       <c r="H49" s="18"/>
     </row>
     <row r="50" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="B50" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="5"/>
       <c r="E50" s="6"/>
       <c r="F50" s="5"/>
       <c r="G50" s="26"/>
-      <c r="H50" s="18"/>
+      <c r="H50" s="18" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="51" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C51" s="6"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="5"/>
       <c r="D51" s="5"/>
-      <c r="E51" s="6"/>
+      <c r="E51" s="5"/>
       <c r="F51" s="5"/>
       <c r="G51" s="26"/>
-      <c r="H51" s="18" t="s">
-        <v>56</v>
-      </c>
+      <c r="H51" s="18"/>
     </row>
     <row r="52" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C52" s="6"/>
+      <c r="B52" s="4"/>
+      <c r="C52" s="5"/>
       <c r="D52" s="5"/>
-      <c r="E52" s="6"/>
+      <c r="E52" s="5"/>
       <c r="F52" s="5"/>
       <c r="G52" s="26"/>
-      <c r="H52" s="18" t="s">
-        <v>58</v>
-      </c>
+      <c r="H52" s="18"/>
     </row>
     <row r="53" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="4"/>
-      <c r="C53" s="5"/>
+      <c r="B53" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C53" s="6"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
+      <c r="E53" s="6"/>
       <c r="F53" s="5"/>
       <c r="G53" s="26"/>
       <c r="H53" s="18"/>
     </row>
     <row r="54" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="B54" s="4" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
+      <c r="E54" s="6"/>
       <c r="F54" s="5"/>
       <c r="G54" s="26"/>
-      <c r="H54" s="18"/>
+      <c r="H54" s="18" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="55" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="5"/>
@@ -1762,14 +1953,12 @@
       <c r="F55" s="5"/>
       <c r="G55" s="26"/>
       <c r="H55" s="18" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" s="6"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -1777,30 +1966,43 @@
       <c r="H56" s="18"/>
     </row>
     <row r="57" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="B57" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="5"/>
       <c r="E57" s="6"/>
       <c r="F57" s="5"/>
-      <c r="G57" s="26"/>
+      <c r="G57" s="26" t="s">
+        <v>71</v>
+      </c>
       <c r="H57" s="18" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="4"/>
-      <c r="C58" s="5"/>
+      <c r="B58" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C58" s="6"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
+      <c r="E58" s="6"/>
       <c r="F58" s="5"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="18"/>
+      <c r="G58" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="59" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="4"/>
-      <c r="C59" s="5"/>
+      <c r="B59" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" s="6"/>
       <c r="D59" s="5"/>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
@@ -1808,13 +2010,17 @@
       <c r="H59" s="18"/>
     </row>
     <row r="60" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="4"/>
-      <c r="C60" s="5"/>
+      <c r="B60" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="6"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
+      <c r="E60" s="6"/>
       <c r="F60" s="5"/>
       <c r="G60" s="26"/>
-      <c r="H60" s="18"/>
+      <c r="H60" s="18" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="61" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
@@ -1861,9 +2067,36 @@
       <c r="G65" s="26"/>
       <c r="H65" s="18"/>
     </row>
-    <row r="66" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="4"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="26"/>
+      <c r="H66" s="18"/>
+    </row>
+    <row r="67" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="4"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+      <c r="F67" s="5"/>
+      <c r="G67" s="26"/>
+      <c r="H67" s="18"/>
+    </row>
+    <row r="68" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="4"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="5"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="18"/>
+    </row>
+    <row r="69" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>